<commit_message>
updated measurement template measure option
</commit_message>
<xml_diff>
--- a/StateOfPractice/Methodology/Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
+++ b/StateOfPractice/Methodology/Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="147">
   <si>
     <t xml:space="preserve">Metrics &amp; Description</t>
   </si>
@@ -426,6 +426,9 @@
     <t xml:space="preserve">Number of total lines added to text-based files.</t>
   </si>
   <si>
+    <t xml:space="preserve">(number or {not git repo})</t>
+  </si>
+  <si>
     <t xml:space="preserve">Number of total lines deleted from text-based files.</t>
   </si>
   <si>
@@ -435,7 +438,7 @@
     <t xml:space="preserve">Numbers of commits by year in the last 5 years. (Count from as early as possible if the project is younger than 5 years.) </t>
   </si>
   <si>
-    <t xml:space="preserve">(list of numbers)</t>
+    <t xml:space="preserve">(list of numbers or {not git repo})</t>
   </si>
   <si>
     <t xml:space="preserve">Numbers of commits by month in the last 12 months.</t>
@@ -462,7 +465,7 @@
     <t xml:space="preserve">Number of stars.</t>
   </si>
   <si>
-    <t xml:space="preserve">({number, n/a})</t>
+    <t xml:space="preserve">(number or {n/a})</t>
   </si>
   <si>
     <t xml:space="preserve">Number of forks.</t>
@@ -718,15 +721,15 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AS139" activeCellId="0" sqref="AS139"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A95" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="H95" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
+      <selection pane="topRight" activeCell="H111" activeCellId="0" sqref="H111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="1" width="26.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.71"/>
@@ -2826,7 +2829,7 @@
         <v>128</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
       <c r="D108" s="7"/>
       <c r="F108" s="7"/>
@@ -2844,10 +2847,10 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D109" s="7"/>
       <c r="F109" s="7"/>
@@ -2865,10 +2868,10 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
       <c r="D110" s="7"/>
       <c r="F110" s="7"/>
@@ -2886,10 +2889,10 @@
     </row>
     <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D111" s="7"/>
       <c r="F111" s="7"/>
@@ -2907,10 +2910,10 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="D112" s="7"/>
       <c r="F112" s="7"/>
@@ -2929,7 +2932,7 @@
     </row>
     <row r="113" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
@@ -2979,7 +2982,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>12</v>
@@ -3005,7 +3008,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>12</v>
@@ -3031,7 +3034,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>12</v>
@@ -3057,7 +3060,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>12</v>
@@ -3083,7 +3086,7 @@
     </row>
     <row r="119" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
@@ -3107,42 +3110,42 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
updated measurement template constants question, related methodology section 9 comment, and section2 status
</commit_message>
<xml_diff>
--- a/StateOfPractice/Methodology/Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
+++ b/StateOfPractice/Methodology/Combined_MeasurementTemplate_EmpiricalMeasures.xlsx
@@ -721,13 +721,13 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A95" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="H95" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
-      <selection pane="topRight" activeCell="H111" activeCellId="0" sqref="H111"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="H78" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A78" activeCellId="0" sqref="A78"/>
+      <selection pane="topRight" activeCell="B88" activeCellId="0" sqref="B88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.87"/>
@@ -2426,7 +2426,7 @@
         <v>113</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>

</xml_diff>